<commit_message>
Start writing the search string into blocks, download records from WOS for the general options
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General options" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="126">
   <si>
     <t>WOS Core Collection (Bibliotheque La Perouse Access)</t>
   </si>
@@ -89,9 +89,6 @@
     <t>TS = (estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR "inter tidal" OR "sub tidal" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")</t>
   </si>
   <si>
-    <t>Entire ocean-related block</t>
-  </si>
-  <si>
     <t>Block</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>TS = (climat* NEAR/2 (mitigat* OR adapt* OR resilien*))</t>
   </si>
   <si>
-    <t>TS = (emission$ OR [carbon keywords] OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon*)</t>
-  </si>
-  <si>
     <t>TS = (efficien* OR sustainab* OR alternat* OR electric OR "negative emission$" OR decarboni?e OR "carbon neutral" OR (reduc* NEAR/1 "carbon footprint"))</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>TS = (OTEC OR (((wind NEAR/1 offshore) OR offshore OR wave OR tide OR tidal OR current OR thermohaline OR thermal OR "salinity gradient$" OR solar OR photovoltaic OR geothermal) NEAR/5 (energ* OR power OR technolog* OR panel$ OR array$ OR farm$)))</t>
   </si>
   <si>
-    <t>Add NO TERMS for option types we do not consider</t>
-  </si>
-  <si>
     <t>Ocean-related + climate change + option NEAR/5 MIT_ADAPT NOT NO_TERMS</t>
   </si>
   <si>
@@ -393,6 +384,24 @@
   </si>
   <si>
     <t>Between all the chunks, all of the test list articles are retreived</t>
+  </si>
+  <si>
+    <t>DO = (10.2989/16085914.2016.1146122 OR 10.1007/s13280-022-01811-2 OR 10.1146/annurev-marine-010318-095300 OR 10.1016/j.apenergy.2020.114515 OR 10.1016/j.apenergy.2016.07.070 OR 10.1002/aqc.2809 OR 10.5194/bg-6-901-2009 OR 10.1016/j.biocon.2021.109107 OR 10.1016/j.biocon.2019.05.005 OR 10.1038/s43247-022-00625-0 OR 10.1111/conl.12587 OR 10.1111/conl.12217 OR 10.1016/j.cub.2021.01.070 OR 10.1007/s40641-020-00161-z OR 10.3390/d12060245 OR 10.5194/esd-9-339-2018 OR 10.1002/eap.2650 OR 10.1016/j.ecoleng.2021.106255 OR 10.1016/j.ecoleng.2017.05.031 OR 10.1016/j.ecoleng.2015.09.016 OR 10.1111/ele.12598 OR 10.1080/20964129.2022.2101547 OR 10.1016/j.ecoser.2022.101429 OR 10.1039/d0ee03757e OR 10.1007/s10668-020-01013-4 OR 10.1088/1748-9326/11/11/113001 OR 10.1088/1748-9326/11/7/074008 OR 10.1088/1748-9326/9/4/044009 OR 10.1007/s11356-017-8749-3 OR 10.1016/j.ecss.2017.09.007 OR 10.1111/faf.12595 OR 10.3389/fmars.2022.802762 OR 10.3389/fmars.2020.00097 OR 10.3389/fmars.2019.00263 OR 10.3389/fmars.2019.00146 OR 10.3389/fmars.2018.00337 OR 10.1029/2010GL045489 OR 10.1029/2009GL041961 OR 10.1029/2005GB002591 OR 10.1111/gcb.16105 OR 10.1007/s10750-014-2157-1 OR 10.1093/icesjms/fsab146 OR 10.1093/icesjms/fsz038 OR 10.1111/1365-2664.13683 OR 10.1111/j.1365-2664.2009.01697.x OR 10.1016/j.jclepro.2021.127814 OR 10.1111/jfr3.12567 OR 10.1029/2021JG006573 OR 10.1002/2017JG004336 OR 10.1063/5.0069452 OR 10.1002/lno.12063 OR 10.1002/lno.10128 OR 10.3354/meps12929 OR 10.3354/meps12652 OR 10.1016/j.marpol.2022.105262 OR 10.1016/j.marpol.2022.104996 OR 10.1111/mec.15482 OR 10.1111/mec.15364 OR 10.1038/nature17155 OR 10.1038/s41558-017-0065-x OR 10.1038/NCLIMATE1463 OR 10.1038/s41467-021-22837-2 OR 10.1038/s41467-019-12176-8 OR 10.1038/ncomms4304 OR 10.1038/s41559-022-01722-1 OR 10.1038/s41565-022-01226-w OR 10.1038/s43017-021-00224-1 OR 10.1038/s43017-021-00214-3 OR 10.1016/j.ocecoaman.2017.07.005 OR 10.1016/j.oceaneng.2015.11.022 OR 10.1016/j.oceaneng.2015.01.013 OR 10.1016/j.oneear.2022.09.002 OR 10.1016/j.oneear.2022.04.005 OR 10.1371/journal.pone.0224347 OR 10.1073/pnas.1721415116 OR 10.1073/pnas.1701262114 OR 10.1073/pnas.1611056113 OR 10.1007/s10113-020-01691-w OR 10.1007/s10113-020-01699-2 OR 10.1007/s10113-017-1256-8 OR 10.1016/j.renene.2021.08.052 OR 10.1111/rec.13498 OR 10.1111/rec.13069 OR 10.1111/j.1526-100X.2005.00062.x OR 10.1126/science.284.5416.943 OR 10.1126/sciadv.abg3088 OR 10.1126/sciadv.aba2498 OR 10.1126/sciadv.aax8995 OR 10.1126/sciadv.aao1378 OR 10.1016/j.scitotenv.2022.153803 OR 10.1038/s41598-022-18668-w OR 10.1038/s41598-022-18109-8 OR 10.1038/s41598-020-77885-3 OR 10.1038/s41598-020-69258-7 OR 10.1038/s41598-019-44925-6 OR 10.1007/s11625-019-00722-8 OR 10.5194/wes-7-801-2022)</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LA=(English)</t>
+  </si>
+  <si>
+    <t>Entire ocean-related block retreives all articles, but number of search results is too large</t>
+  </si>
+  <si>
+    <t>TS = (emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon*)</t>
+  </si>
+  <si>
+    <t>Add NO TERMS -- does not change the number of test list results</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -479,6 +488,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,33 +785,35 @@
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="9" max="9" width="24.54296875" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" customWidth="1"/>
-    <col min="12" max="12" width="26.453125" customWidth="1"/>
+    <col min="10" max="10" width="6.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+    <col min="14" max="14" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -815,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -824,45 +837,90 @@
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="16">
+        <v>44953</v>
+      </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4">
+        <v>89</v>
+      </c>
+      <c r="M4">
+        <v>1899526</v>
+      </c>
+      <c r="N4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="16">
+        <v>44953</v>
+      </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5">
+        <v>71</v>
+      </c>
+      <c r="M5">
+        <v>559792</v>
+      </c>
+      <c r="N5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="16">
+        <v>44953</v>
+      </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6">
+        <v>97</v>
+      </c>
+      <c r="M6">
+        <v>1898637</v>
+      </c>
+      <c r="N6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>44953</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -870,148 +928,290 @@
       <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="K7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="3">
+        <v>63</v>
+      </c>
+      <c r="M7" s="3">
+        <v>110146</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="4">
+        <v>23</v>
+      </c>
+      <c r="M8" s="4">
+        <v>6948</v>
+      </c>
+      <c r="N8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="4">
+        <v>39</v>
+      </c>
+      <c r="M9" s="4">
+        <v>225088</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="L8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="K10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="4">
+        <v>27</v>
+      </c>
+      <c r="M10" s="4">
+        <v>213181</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="K11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="4">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4">
+        <v>22641</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="L10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="K12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="4">
+        <v>25</v>
+      </c>
+      <c r="M12" s="4">
+        <v>55555</v>
+      </c>
+      <c r="N12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="L11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="K13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="4">
+        <v>8</v>
+      </c>
+      <c r="M13" s="4">
+        <v>52564</v>
+      </c>
+      <c r="N13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="L12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="K14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="4">
+        <v>22</v>
+      </c>
+      <c r="M14" s="4">
+        <v>40004</v>
+      </c>
+      <c r="N14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="16">
+        <v>44953</v>
+      </c>
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
-      <c r="L15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="4">
+        <v>88</v>
+      </c>
+      <c r="M15" s="4">
+        <v>536102</v>
+      </c>
+      <c r="N15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="17">
+        <v>44953</v>
+      </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F16"/>
-      <c r="G16" t="s">
+      <c r="G16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="3">
+        <v>73</v>
+      </c>
+      <c r="M16" s="3">
+        <v>249382</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
         <v>44</v>
       </c>
-      <c r="H16"/>
-      <c r="L16" s="3" t="s">
+      <c r="K17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="4">
+        <v>54</v>
+      </c>
+      <c r="M17" s="4">
+        <v>58087</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="16">
+        <v>44953</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="K18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="4">
+        <v>29</v>
+      </c>
+      <c r="M18" s="4">
+        <v>15135</v>
+      </c>
+      <c r="N18" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="4" t="s">
+    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="17">
+        <v>44953</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>12</v>
@@ -1020,13 +1220,22 @@
         <v>18</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>51</v>
+      <c r="K19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="3">
+        <v>29</v>
+      </c>
+      <c r="M19" s="3">
+        <v>14069</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1036,41 +1245,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="6.36328125" customWidth="1"/>
     <col min="5" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="7.54296875" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1088,41 +1300,56 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="16">
+        <v>44953</v>
+      </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="16">
+        <v>44953</v>
+      </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="s">
-        <v>56</v>
+      <c r="L5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1385,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1166,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1181,7 +1408,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -1201,7 +1428,7 @@
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1210,54 +1437,54 @@
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -1266,83 +1493,83 @@
         <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1601,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1382,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1397,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -1417,7 +1644,7 @@
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1426,32 +1653,32 @@
         <v>18</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>12</v>
@@ -1461,32 +1688,32 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -1496,27 +1723,27 @@
         <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C9" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1775,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1556,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1571,13 +1798,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>6</v>
@@ -1597,7 +1824,7 @@
     </row>
     <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1607,33 +1834,33 @@
         <v>18</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1642,123 +1869,123 @@
         <v>18</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
@@ -1767,143 +1994,143 @@
         <v>18</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="3:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I21" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>13</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +2165,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1946,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1966,7 +2193,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish scoping searches by block
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General options" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="116">
   <si>
     <t>WOS Core Collection (Bibliotheque La Perouse Access)</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Ocean-related + climate change + option NEAR/5 MIT_ADAPT</t>
   </si>
   <si>
-    <t>OPTION NEAR/5 MIT_ADAPT</t>
-  </si>
-  <si>
     <t>TS = (option$ OR manage* OR measure$ OR action$ OR approach* OR pathway$ OR solution$ OR strateg* OR policies OR policy OR practi?e$ OR intervention$ OR technol* OR opportunit* OR "geo engineering" OR "climate engineering" OR "eco engineering")</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>TS = (OTEC OR (((wind NEAR/1 offshore) OR offshore OR wave OR tide OR tidal OR current OR thermohaline OR thermal OR "salinity gradient$" OR solar OR photovoltaic OR geothermal) NEAR/5 (energ* OR power OR technolog* OR panel$ OR array$ OR farm$)))</t>
   </si>
   <si>
-    <t>Ocean-related + climate change + option NEAR/5 MIT_ADAPT NOT NO_TERMS</t>
-  </si>
-  <si>
     <t>Ocean-related and renewable</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>97 total</t>
   </si>
   <si>
-    <t>Add in NOT terms</t>
-  </si>
-  <si>
     <t>INTERVENTION_MIT</t>
   </si>
   <si>
@@ -278,36 +269,6 @@
     <t xml:space="preserve">TS = ("environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR "blue carbon" OR "natural carbon sink$" OR "intervention ecology" OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat* OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) AND (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function"))) </t>
   </si>
   <si>
-    <t>General built infrastructure</t>
-  </si>
-  <si>
-    <t>protection &amp; beach/shore nourishment</t>
-  </si>
-  <si>
-    <t>early warning systems</t>
-  </si>
-  <si>
-    <t>accomodation &amp; relocation</t>
-  </si>
-  <si>
-    <t>TS = ((infrastructure NEAR/2 (green OR natural OR blue OR ecological)) OR "climate buffer$" OR technolog* OR seawall$ OR "sea wall$" OR ((coast* OR sea OR hard) NEAR/1 defense$) OR breakwater OR "rip?rap" OR jetty OR jetties OR "ground elev*" OR reclaim OR reclamation OR "land rais*" OR (rain* NEAR/1 harvest*) OR (groundwater NEAR/1 pump*) OR desalinisation OR desalination OR "storm surge gate$" OR "flood barrier$" OR dyke$ OR dike$ OR engineering OR urbani$ation OR infrastructure OR development$ OR "built structure$" OR "artificial structure$" OR "artificial reef$" OR "artificial island$")</t>
-  </si>
-  <si>
-    <t>TS = (relocat* OR "spatial planning" OR (development NEAR/2 plan*) OR "integrated coastal management")</t>
-  </si>
-  <si>
-    <t>TS = ((beach OR shore* OR coast*) NEAR/2 (nourish* OR protect*))</t>
-  </si>
-  <si>
-    <t>TS = (alert* OR warn* OR cris?s OR evacuat*)</t>
-  </si>
-  <si>
-    <t>TS = (forecast* OR "monitor* system$")</t>
-  </si>
-  <si>
-    <t>monitoring systems &amp; forecasts</t>
-  </si>
-  <si>
     <t>all terms</t>
   </si>
   <si>
@@ -335,54 +296,9 @@
     <t>Socio-institutional</t>
   </si>
   <si>
-    <t>knowledge diversity</t>
-  </si>
-  <si>
-    <t>livlihood diversification</t>
-  </si>
-  <si>
-    <t>ensuring mobility and migration</t>
-  </si>
-  <si>
-    <t>finance and market mechanisms</t>
-  </si>
-  <si>
-    <t>disaster response</t>
-  </si>
-  <si>
-    <t>ocean governance</t>
-  </si>
-  <si>
-    <t>socially inclusive policies and participation</t>
-  </si>
-  <si>
-    <t>TS = (((knowledge) NEAR/1 (divers* OR indigenous OR communit*)))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS = ((econom* OR finance OR commerc* OR livelihood* OR industr* OR fisher* OR aquaculture OR mariculture OR farm* OR touris* OR product* OR consumer* OR subsist* OR tradition* OR indig*) AND (diversif* OR sustainabl* OR relocat* OR retreat* OR migra* OR resettle* OR displace* OR protect* OR accomodat* OR adapt* resilie* OR ((reduc*) NEAR/2 (vulnerab* OR risk$ OR exposure))) OR "offshore *culture") </t>
-  </si>
-  <si>
-    <t>TS = ("managed retreat" OR move OR migrate OR migration OR retreat OR resettle* OR displace*)</t>
-  </si>
-  <si>
-    <t>TS = (policy OR policies OR practice$ OR practise$ OR "climate change mainstream*")</t>
-  </si>
-  <si>
-    <t>TS = ("economic policy instruments" OR "capital management" OR "market mechanism$" OR "carbon market$" OR "carbon credit$" OR  invest* OR incentiv*)</t>
-  </si>
-  <si>
-    <t>TS = ((respond OR respons*) NEAR/1 (disaster OR risk$ OR extreme$ OR storm$ OR flood$ OR cyclone$ OR "coastal flood$"))</t>
-  </si>
-  <si>
-    <t>TS = (legislat* OR law OR legal* OR rule$ OR regulat* OR litigat* OR govern* OR legislation OR institution* OR "transboundary agreement$")</t>
-  </si>
-  <si>
     <t>TS = (((knowledge) NEAR/1 (divers* OR indigenous OR communit*)) OR policy OR policies OR practice$ OR practise$ OR "climate change mainstream*" OR (econom* OR finance OR commerc* OR livelihood* OR industr* OR fisher* OR aquaculture OR mariculture OR farm* OR touris* OR product* OR consumer* OR subsist* OR tradition* OR indig*) AND (diversif* OR sustainabl* OR relocat* OR retreat* OR migra* OR resettle* OR displace* OR protect* OR accomodat* OR adapt* resilie* OR ((reduc*) NEAR/2 (vulnerab* OR risk$ OR exposure))) OR "offshore *culture" OR "managed retreat" OR move OR migrate OR migration OR retreat OR resettle* OR displace* OR "economic policy instruments" OR "capital management" OR "market mechanism$" OR "carbon market$" OR "carbon credit$" OR  invest* OR incentiv* OR ((respond OR respons*) NEAR/1 (disaster OR risk$ OR extreme$ OR storm$ OR flood$ OR cyclone$ OR "coastal flood$")) OR legislat* OR law OR legal* OR rule$ OR regulat* OR litigat* OR govern* OR legislation OR institution* OR "transboundary agreement$")</t>
   </si>
   <si>
-    <t>Entire string</t>
-  </si>
-  <si>
     <t>Between all the chunks, all of the test list articles are retreived</t>
   </si>
   <si>
@@ -402,6 +318,60 @@
   </si>
   <si>
     <t>Add NO TERMS -- does not change the number of test list results</t>
+  </si>
+  <si>
+    <t>Add in NOT terms -- no test list articles lost</t>
+  </si>
+  <si>
+    <t>TS = (((eutrophication OR oligotrophication OR (oligotrophic* NEAR/1 increas*) OR run-off OR runoff OR "oil spill*" OR ((bio-plastic$ OR bioplastic$ OR microplastic$ OR plastic$) NEAR/5 (pollut*)))OR(climat* NEAR/5 ("risk assess*" OR "vulnerab* assess*" OR "impact assess*"))OR(paleo* OR Holocene)) OR "waste management" OR ozone)</t>
+  </si>
+  <si>
+    <t>add not terms, and add wastewater and ozone</t>
+  </si>
+  <si>
+    <t>TS = ("environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR "blue carbon" OR ((restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat*) NEAR/5 ("natural carbon sink$" OR estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "intervention ecology" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) NEAR/5 (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function")))</t>
+  </si>
+  <si>
+    <t>check if this one returns enough when weighed against the others</t>
+  </si>
+  <si>
+    <t>All nature</t>
+  </si>
+  <si>
+    <t>TS = (((assisted OR artificial OR induced OR manage* OR restor* OR selective OR enhanc*) NEAR/5 (evolution OR adapt* OR migration OR "transgenerational acclimatization" OR breed* OR genetic OR tolerance OR resilien*)) OR "ecosystem pushing" OR "habitat-forming species" OR (species NEAR/10 (relocat* OR translocat*)) OR ((genetic OR population OR ecological) NEAR/5 connectivity) OR "evolutionary rescue" OR "gene drive" OR (restor* NEAR/1 demograph*) OR ((probiotic$ OR phage OR viral) NEAR/1 therap*) OR "ex-situ spawn*" OR "pathogen control" OR protect* OR conserv* OR monitor* OR "climate refug*" OR "natural resource$" OR "natural capital" OR "no-regret" OR (("nature-based" OR "nature based" OR "ecosystem-based" OR "ecosystem based" OR "natural climate") NEAR/2 (solution$ OR approach* OR action$ OR measure$ OR option$)) OR ((sustainable OR "ecosystem-based" OR adaptive OR spatial OR integrated OR "natural resource" OR integrated OR fishery OR fisheries) NEAR/1 management) OR (management NEAR/1 (estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR "inter tidal" OR "sub tidal" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "sustainable ocean economic zones" OR "marine protected area$" OR MPA$ OR ((reduce OR minimize OR minimise OR decrease) AND (disturbance OR loss OR degradation OR overexploit*)) OR "environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR "blue carbon" OR ((restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat*) NEAR/5 ("natural carbon sink$" OR estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "intervention ecology" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) NEAR/5 (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function")))</t>
+  </si>
+  <si>
+    <t>All Societal</t>
+  </si>
+  <si>
+    <t>TS = ((infrastructure NEAR/2 (green OR natural OR blue OR ecological)) OR "climate buffer$" OR technolog* OR seawall$ OR "sea wall$" OR ((coast* OR sea OR hard) NEAR/1 defense$) OR breakwater OR "rip?rap" OR jetty OR jetties OR "ground elev*" OR reclaim OR reclamation OR "land rais*" OR (rain* NEAR/1 harvest*) OR (groundwater NEAR/1 pump*) OR desalinisation OR desalination OR "storm surge gate$" OR "flood barrier$" OR dyke$ OR dike$ OR engineering OR urbani$ation OR infrastructure OR development$ OR "built structure$" OR "artificial structure$" OR "artificial reef$" OR "artificial island$" OR relocat* OR "spatial planning" OR (development NEAR/2 plan*) OR "integrated coastal management" OR ((beach OR shore* OR coast*) NEAR/2 (nourish* OR protect*)) OR alert* OR warn* OR cris?s OR evacuat* OR forecast* OR "monitor* system$" OR ((knowledge) NEAR/1 (divers* OR indigenous OR communit*)) OR policy OR policies OR practice$ OR practise$ OR "climate change mainstream*" OR (econom* OR finance OR commerc* OR livelihood* OR industr* OR fisher* OR aquaculture OR mariculture OR farm* OR touris* OR product* OR consumer* OR subsist* OR tradition* OR indig*) AND (diversif* OR sustainabl* OR relocat* OR retreat* OR migra* OR resettle* OR displace* OR protect* OR accomodat* OR adapt* resilie* OR ((reduc*) NEAR/2 (vulnerab* OR risk$ OR exposure))) OR "offshore *culture" OR "managed retreat" OR move OR migrate OR migration OR retreat OR resettle* OR displace* OR "economic policy instruments" OR "capital management" OR "market mechanism$" OR "carbon market$" OR "carbon credit$" OR  invest* OR incentiv* OR ((respond OR respons*) NEAR/1 (disaster OR risk$ OR extreme$ OR storm$ OR flood$ OR cyclone$ OR "coastal flood$")) OR legislat* OR law OR legal* OR rule$ OR regulat* OR litigat* OR govern* OR legislation OR institution* OR "transboundary agreement$")</t>
+  </si>
+  <si>
+    <t>Might not be worth all the extra terms to reduce by only 3,000 records -- just keep the general block</t>
+  </si>
+  <si>
+    <t>GENERAL_OPTION</t>
+  </si>
+  <si>
+    <t>INTERVENTION Formula = TS = ((OCEAN_RENEWABLE) OR ((CLIMATE_CHANGE) AND ((GENERAL_OPTION) OR (INTERVENTION_MIT) OR (INTERVENTION_NAT) OR (SOC_ADAPT))))</t>
+  </si>
+  <si>
+    <t>All mitigation</t>
+  </si>
+  <si>
+    <t>TS = (((clean OR renew*) NEAR/5 (fuel$ OR coal OR diesel OR hydrogen OR energ* OR power OR technolog*)) OR "iron salt aerosol$" OR "methane oxidation" OR biofuel$ OR energ* OR ((efficien* OR sustainab* OR alternat*) NEAR/5 (transport OR ship* OR biotechnolog* OR feed$ OR aquafeed$ OR (supply NEAR/2 chain$) OR product$ OR production OR material$)) OR "integrated multitrophic aquaculture" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) NEAR/15 (capture OR uptake OR remov* OR drawdown OR extract* OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)) OR CCS OR DACCS OR "secure seafloor container storage" OR "bio energy" OR bioenergy OR (biomass NEAR/2 energy) OR biochar OR (bio* NEAR/2 charcoal) OR ((seaweed OR "sea weed" OR macroalga$ OR biomass OR crop$ OR log$) NEAR/2 (soil OR agriculture OR pyrolysis OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)))</t>
+  </si>
+  <si>
+    <t>TS = (((assisted OR artificial OR induced OR manage* OR restor* OR selective OR enhanc*) NEAR/5 (evolution OR adapt* OR migration OR "transgenerational acclimatization" OR breed* OR genetic OR tolerance OR resilien*)) OR "ecosystem pushing" OR "habitat-forming species" OR (species NEAR/10 (relocat* OR translocat*)) OR ((genetic OR population OR ecological) NEAR/5 connectivity) OR "evolutionary rescue" OR "gene drive" OR (restor* NEAR/1 demograph*) OR ((probiotic$ OR phage OR viral) NEAR/1 therap*) OR "ex-situ spawn*" OR "pathogen control" OR protect* OR conserv* OR monitor* OR "climate refug*" OR "natural resource$" OR "natural capital" OR "no-regret" OR (("nature-based" OR "nature based" OR "ecosystem-based" OR "ecosystem based" OR "natural climate") NEAR/2 (solution$ OR approach* OR action$ OR measure$ OR option$)) OR ((sustainable OR "ecosystem-based" OR adaptive OR spatial OR integrated OR "natural resource" OR integrated OR fishery OR fisheries) NEAR/1 management) OR (management NEAR/1 (estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR "inter tidal" OR "sub tidal" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "sustainable ocean economic zones" OR "marine protected area$" OR MPA$ OR ((reduce OR minimize OR minimise OR decrease) AND (disturbance OR loss OR degradation OR overexploit*)) OR "environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR "blue carbon" OR "natural carbon sink$" OR "intervention ecology" OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat* OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) AND (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function")))</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND ((OCEAN_RENEWABLE) OR ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) OR ((CLIMATE_CHANGE) AND ((INTERVENTION_MIT) OR (INTERVENTION_NAT) OR (SOC_ADAPT)))) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>FORMULA TS=</t>
+  </si>
+  <si>
+    <t>All general option block</t>
   </si>
 </sst>
 </file>
@@ -431,15 +401,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -465,11 +441,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -481,15 +468,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +770,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,12 +797,12 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -828,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -840,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -853,7 +850,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>44953</v>
       </c>
       <c r="B4" t="s">
@@ -863,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="L4">
         <v>89</v>
@@ -876,7 +873,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>44953</v>
       </c>
       <c r="C5" t="s">
@@ -896,7 +893,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
+      <c r="A6" s="13">
         <v>44953</v>
       </c>
       <c r="C6" t="s">
@@ -912,11 +909,11 @@
         <v>1898637</v>
       </c>
       <c r="N6" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17">
+      <c r="A7" s="14">
         <v>44953</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -942,7 +939,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="16">
+      <c r="A8" s="13">
         <v>44953</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -965,14 +962,14 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="16">
+      <c r="A9" s="13">
         <v>44953</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>39</v>
@@ -988,7 +985,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>44953</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1008,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>44953</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1034,7 +1031,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>44953</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1057,7 +1054,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="16">
+      <c r="A13" s="13">
         <v>44953</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1080,7 +1077,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="16">
+      <c r="A14" s="13">
         <v>44953</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1103,7 +1100,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="16">
+      <c r="A15" s="13">
         <v>44953</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1126,7 +1123,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
+      <c r="A16" s="14">
         <v>44953</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1139,7 +1136,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>39</v>
@@ -1151,21 +1148,21 @@
         <v>249382</v>
       </c>
       <c r="N16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="13">
+        <v>44953</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
-        <v>44953</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>39</v>
@@ -1177,21 +1174,21 @@
         <v>58087</v>
       </c>
       <c r="N17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="13">
+        <v>44953</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
-        <v>44953</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" t="s">
-        <v>46</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>39</v>
@@ -1203,15 +1200,15 @@
         <v>15135</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17">
+      <c r="A19" s="14">
         <v>44953</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>12</v>
@@ -1220,10 +1217,10 @@
         <v>18</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="I19" t="s">
+        <v>99</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>39</v>
@@ -1235,7 +1232,7 @@
         <v>14069</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1247,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,7 +1271,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1303,7 +1300,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -1316,28 +1313,34 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>44953</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
+        <v>94</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>43845</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>44953</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1346,10 +1349,19 @@
         <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>99</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>42840</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1360,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:E8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1371,24 +1383,24 @@
     <col min="7" max="7" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1408,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -1417,18 +1429,27 @@
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15">
+        <v>44953</v>
+      </c>
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1437,139 +1458,272 @@
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="6">
+        <v>10</v>
+      </c>
+      <c r="M4" s="6">
+        <v>69864</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>14412</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6">
+        <v>13</v>
+      </c>
+      <c r="M6">
+        <v>80198</v>
+      </c>
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>44953</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7">
+        <v>13</v>
+      </c>
+      <c r="M7">
+        <v>76264</v>
+      </c>
+      <c r="N7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <v>44953</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="3">
+        <v>28</v>
+      </c>
+      <c r="M8" s="3">
+        <v>53978</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="4" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="4">
+        <v>9</v>
+      </c>
+      <c r="M9" s="4">
+        <v>7362</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="3" t="s">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="4">
+        <v>8</v>
+      </c>
+      <c r="M10" s="4">
+        <v>57219</v>
+      </c>
+      <c r="N10" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="4">
+        <v>16</v>
+      </c>
+      <c r="M11" s="4">
+        <v>8298</v>
+      </c>
+      <c r="N11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="4">
+        <v>36</v>
+      </c>
+      <c r="M12" s="4">
+        <v>104581</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24">
+        <v>44953</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="25">
+        <v>36</v>
+      </c>
+      <c r="M13" s="25">
+        <v>84923</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26">
+        <v>44953</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>68</v>
+      <c r="G15" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="27">
+        <v>38</v>
+      </c>
+      <c r="M15" s="27">
+        <v>116438</v>
       </c>
     </row>
   </sheetData>
@@ -1579,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,7 +1755,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1624,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -1644,7 +1798,7 @@
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1653,10 +1807,16 @@
         <v>18</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="6">
+        <v>12</v>
+      </c>
+      <c r="K4" s="6">
+        <v>7199</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1669,16 +1829,22 @@
       <c r="G5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>13</v>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="8">
+        <v>12</v>
+      </c>
+      <c r="K5" s="8">
+        <v>6784</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>12</v>
@@ -1688,10 +1854,16 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="J6">
+        <v>53</v>
+      </c>
+      <c r="K6">
+        <v>100845</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1704,16 +1876,22 @@
       <c r="G7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>13</v>
+      <c r="I7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="8">
+        <v>53</v>
+      </c>
+      <c r="K7" s="8">
+        <v>94162</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -1723,27 +1901,104 @@
         <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="J8" s="4">
+        <v>44</v>
+      </c>
+      <c r="K8" s="4">
+        <v>102017</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="6">
+        <v>44</v>
+      </c>
+      <c r="K9" s="6">
+        <v>80731</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="4">
+        <v>31</v>
+      </c>
+      <c r="K10" s="4">
+        <v>47190</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="4">
+        <v>31</v>
+      </c>
+      <c r="K11" s="4">
+        <v>37785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="16">
+        <v>64</v>
+      </c>
+      <c r="K14" s="16">
+        <v>125353</v>
       </c>
     </row>
   </sheetData>
@@ -1753,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:N3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1775,7 +2030,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1798,13 +2053,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>6</v>
@@ -1822,9 +2077,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
-        <v>99</v>
+    <row r="4" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17">
+        <v>44953</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1833,34 +2091,52 @@
       <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="10" t="s">
+      <c r="G4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="10">
+        <v>31</v>
+      </c>
+      <c r="M4" s="10">
+        <v>13071</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19">
+        <v>44953</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>95</v>
+      <c r="L5" s="23">
+        <v>31</v>
+      </c>
+      <c r="M5" s="22">
+        <v>12345</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18">
+        <v>44953</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1868,332 +2144,207 @@
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>98</v>
+      <c r="G6" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="3">
+        <v>19</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7742</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>44953</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
         <v>88</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>7231</v>
+      </c>
+      <c r="N7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
+        <v>44953</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="N8" t="s">
+      <c r="L8" s="3">
+        <v>25</v>
+      </c>
+      <c r="M8" s="3">
+        <v>8889</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
+        <v>44953</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="6">
+        <v>25</v>
+      </c>
+      <c r="M9" s="6">
+        <v>8324</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18">
+        <v>44953</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
-        <v>91</v>
-      </c>
-      <c r="N9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
-        <v>92</v>
-      </c>
-      <c r="N10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
-        <v>100</v>
-      </c>
-      <c r="N11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
-        <v>101</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="I10" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="K10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="3">
+        <v>28</v>
+      </c>
+      <c r="M10" s="3">
+        <v>10239</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="N20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="I21" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="8.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G4" t="s">
-        <v>119</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>44953</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5">
+        <v>97</v>
+      </c>
+      <c r="D5">
+        <v>296565</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to add more specificity to each block, e.g. modifying the climate change string for each block
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General options" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="145">
   <si>
     <t>WOS Core Collection (Bibliotheque La Perouse Access)</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Test list DOIS</t>
   </si>
   <si>
-    <t>DO = (</t>
-  </si>
-  <si>
     <t>TS = ("climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR (climat* NEAR/2 (mitigat* OR adapt* OR resilien*)) emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR efficien* OR sustainab* OR alternat* OR electric OR "negative emission$" OR decarboni?e OR "carbon neutral" OR (reduc* NEAR/1 "carbon footprint") OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion" OR heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR acidif* OR "increas* acidity" OR "aragonite saturation" OR pH OR (ris* NEAR/1 "sea level$") OR "coastal flood$" OR "coastal hazard$" OR (("sea water" OR saltwater OR "salt water") NEAR/1 (incursion OR intrusion)) OR salini$ation OR aquifer$ OR (shore* NEAR/1 protect*))</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t>TS = (((clean OR renew*) NEAR/5 (fuel$ OR coal OR diesel OR hydrogen OR energ* OR power OR technolog*)) OR "iron salt aerosol$" OR "methane oxidation" OR biofuel$ OR energ* OR ((efficien* OR sustainab* OR alternat*) NEAR/5 (transport OR ship* OR biotechnolog* OR feed$ OR aquafeed$ OR (supply NEAR/2 chain$) OR product$ OR production OR material$)) OR "integrated multitrophic aquaculture" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) NEAR/15 (capture OR uptake OR remov* OR drawdown OR extract* OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)) OR CCS OR DACCS OR "secure seafloor container storage" OR "bio energy" OR bioenergy OR (biomass NEAR/2 energy) OR biochar OR (bio* NEAR/2 charcoal) OR ((seaweed OR "sea weed" OR macroalga$ OR biomass OR crop$ OR log$) NEAR/2 (soil OR agriculture OR pyrolysis OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)))</t>
   </si>
   <si>
-    <t>TS = (((assisted OR artificial OR induced OR manage* OR restor* OR selective OR enhanc*) NEAR/5 (evolution OR adapt* OR migration OR "transgenerational acclimatization" OR breed* OR genetic OR tolerance OR resilien*)) OR "ecosystem pushing" OR "habitat-forming species" OR (species NEAR/10 (relocat* OR translocat*)) OR ((genetic OR population OR ecological) NEAR/5 connectivity) OR "evolutionary rescue" OR "gene drive" OR (restor* NEAR/1 demograph*) OR ((probiotic$ OR phage OR viral) NEAR/1 therap*) OR "ex-situ spawn*" OR "pathogen control" OR protect* OR conserv* OR monitor* OR "climate refug*" OR "natural resource$" OR "natural capital" OR "no-regret" OR (("nature-based" OR "nature based" OR "ecosystem-based" OR "ecosystem based" OR "natural climate") NEAR/2 (solution$ OR approach* OR action$ OR measure$ OR option$)) OR ((sustainable OR "ecosystem-based" OR adaptive OR spatial OR integrated OR "natural resource" OR integrated OR fishery OR fisheries) NEAR/1 management) OR (management NEAR/1 (estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR "inter tidal" OR "sub tidal" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "sustainable ocean economic zones" OR "marine protected area$" OR MPA$ OR ((reduce OR minimize OR minimise OR decrease) AND (disturbance OR loss OR degradation OR overexploit*)) OR "environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR "blue carbon" OR "natural carbon sink$" OR "intervention ecology" OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat* OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) AND (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function")))</t>
-  </si>
-  <si>
     <t>(OCEAN_RELATED) AND ((OCEAN_RENEWABLE) OR ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) OR ((CLIMATE_CHANGE) AND ((INTERVENTION_MIT) OR (INTERVENTION_NAT) OR (SOC_ADAPT)))) NOT (NO_TERMS)</t>
   </si>
   <si>
@@ -372,6 +366,99 @@
   </si>
   <si>
     <t>All general option block</t>
+  </si>
+  <si>
+    <t>TS = ("climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR (climat* NEAR/2 (mitigat* OR adapt* OR resilien*)) OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR efficien* OR sustainab* OR alternat* OR electric OR "negative emission$" OR decarboni?e OR "carbon neutral" OR (reduc* NEAR/1 "carbon footprint") OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion" OR heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR acidif* OR "increas* acidity" OR "aragonite saturation" OR pH OR (ris* NEAR/1 "sea level$") OR "coastal flood$" OR "coastal hazard$" OR (("sea water" OR saltwater OR "salt water") NEAR/1 (incursion OR intrusion)) OR salini$ation OR aquifer$ OR (shore* NEAR/1 protect*))</t>
+  </si>
+  <si>
+    <t>All mitigation + alter climate change</t>
+  </si>
+  <si>
+    <t>Mitigate emissions</t>
+  </si>
+  <si>
+    <t>TS = (((clean OR renew*) NEAR/5 (fuel$ OR coal OR diesel OR hydrogen OR energ* OR power OR technolog*)) OR "iron salt aerosol$" OR "methane oxidation" OR biofuel$ OR energ* OR ((efficien* OR sustainab* OR alternat*  OR electric OR decarboni?e) NEAR/5 (transport OR ship* OR biotechnolog* OR feed$ OR aquafeed$ OR (supply NEAR/2 chain$) OR product$ OR production OR material$)) OR "integrated multitrophic aquaculture" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) NEAR/15 (capture OR uptake OR remov* OR drawdown OR extract* OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)) OR CCS OR DACCS OR "secure seafloor container storage" OR "bio energy" OR bioenergy OR (biomass NEAR/2 energy) OR biochar OR (bio* NEAR/2 charcoal) OR ((seaweed OR "sea weed" OR macroalga$ OR biomass OR crop$ OR log$) NEAR/2 (soil OR agriculture OR pyrolysis OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)))</t>
+  </si>
+  <si>
+    <t>TS = (((climat* OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "carbon footprint") NEAR/5 (mitigat* OR reduc*)) OR "negative emission$" OR "carbon neutral")</t>
+  </si>
+  <si>
+    <t>TS = ("climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR ((increas* OR ris*) NEAR/1 temperature$))</t>
+  </si>
+  <si>
+    <t>TS = ("climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR ((increas* OR ris*) NEAR/1 temperature$) OR ((climat* OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "carbon footprint") NEAR/5 (mitigat* OR reduc*)) OR "negative emission$" OR "carbon neutral")</t>
+  </si>
+  <si>
+    <t>General CC + mitigate</t>
+  </si>
+  <si>
+    <t>TS = ("climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR ((increas* OR ris*) NEAR/1 temperature$) OR ((climat* OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "carbon footprint") NEAR/5 (mitigat* OR reduc*)) OR "negative emission$" OR "carbon neutral" OR acidif* OR "increas* acidity" OR "aragonite saturation" OR pH)</t>
+  </si>
+  <si>
+    <t>General CC + mitigate + acidification</t>
+  </si>
+  <si>
+    <t>Ocean related + Whole CC block + All Mitigate interventions</t>
+  </si>
+  <si>
+    <t>Try to reduce CC block; start with general climate change/global warming</t>
+  </si>
+  <si>
+    <t>General societal + reduce climate change</t>
+  </si>
+  <si>
+    <t>TS = ((climat* NEAR/2 (adapt* OR resilien*)) OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)))</t>
+  </si>
+  <si>
+    <t>TS = (emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)))</t>
+  </si>
+  <si>
+    <t>add Increase efficiency/reduce emissions</t>
+  </si>
+  <si>
+    <t>Search #</t>
+  </si>
+  <si>
+    <t>TS = (efficien* OR sustainab* OR alternat* OR electric OR "negative emission$" OR decarboni?e OR "carbon neutral" OR (reduc* NEAR/1 "carbon footprint") OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)))</t>
+  </si>
+  <si>
+    <t>TS = ("climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion" OR efficien* OR sustainab* OR alternat* OR electric OR "negative emission$" OR decarboni?e OR "carbon neutral" OR (reduc* NEAR/1 "carbon footprint") OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)))</t>
+  </si>
+  <si>
+    <t>add Climate adaptation -- doesn't add anything -- remove</t>
+  </si>
+  <si>
+    <t>add Emissions to search #11</t>
+  </si>
+  <si>
+    <t>TS = (emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion")</t>
+  </si>
+  <si>
+    <t>add climate threats</t>
+  </si>
+  <si>
+    <t>search 10 + climate threats</t>
+  </si>
+  <si>
+    <t>TS = (heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion")</t>
+  </si>
+  <si>
+    <t>add Ocean warming to search #13</t>
+  </si>
+  <si>
+    <t>TS = (acidif* OR "increas* acidity" OR "aragonite saturation" OR pH OR heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion")</t>
+  </si>
+  <si>
+    <t>add acidification to search #14 -- doesn't add anything remove</t>
+  </si>
+  <si>
+    <t>add sea level rise to search #14</t>
+  </si>
+  <si>
+    <t>TS = ((ris* NEAR/1 "sea level$") OR "coastal flood$" OR "coastal hazard$" OR (("sea water" OR saltwater OR "salt water") NEAR/1 (incursion OR intrusion)) OR salini$ation OR aquifer$ OR (shore* NEAR/1 protect*) OR heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion")</t>
+  </si>
+  <si>
+    <t>NB search #31</t>
   </si>
 </sst>
 </file>
@@ -410,7 +497,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -478,15 +565,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +865,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,12 +892,12 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -810,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -825,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -837,7 +932,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -854,13 +949,13 @@
         <v>44953</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L4">
         <v>89</v>
@@ -877,10 +972,10 @@
         <v>44953</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5">
         <v>71</v>
@@ -889,7 +984,7 @@
         <v>559792</v>
       </c>
       <c r="N5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -900,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6">
         <v>97</v>
@@ -909,7 +1004,7 @@
         <v>1898637</v>
       </c>
       <c r="N6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -917,7 +1012,7 @@
         <v>44953</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -926,7 +1021,7 @@
         <v>14</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" s="3">
         <v>63</v>
@@ -935,7 +1030,7 @@
         <v>110146</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -943,13 +1038,13 @@
         <v>44953</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" s="4">
         <v>23</v>
@@ -958,7 +1053,7 @@
         <v>6948</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -966,13 +1061,13 @@
         <v>44953</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="4">
         <v>39</v>
@@ -981,7 +1076,7 @@
         <v>225088</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -989,13 +1084,13 @@
         <v>44953</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="4">
         <v>27</v>
@@ -1004,7 +1099,7 @@
         <v>213181</v>
       </c>
       <c r="N10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1012,13 +1107,13 @@
         <v>44953</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" s="4">
         <v>9</v>
@@ -1027,7 +1122,7 @@
         <v>22641</v>
       </c>
       <c r="N11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1035,13 +1130,13 @@
         <v>44953</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="4">
         <v>25</v>
@@ -1050,7 +1145,7 @@
         <v>55555</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1058,13 +1153,13 @@
         <v>44953</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="4">
         <v>8</v>
@@ -1073,7 +1168,7 @@
         <v>52564</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1081,13 +1176,13 @@
         <v>44953</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="4">
         <v>22</v>
@@ -1096,7 +1191,7 @@
         <v>40004</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1104,13 +1199,13 @@
         <v>44953</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="4">
         <v>88</v>
@@ -1119,7 +1214,7 @@
         <v>536102</v>
       </c>
       <c r="N15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1127,19 +1222,19 @@
         <v>44953</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>18</v>
+      <c r="E16" t="s">
+        <v>114</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" s="3">
         <v>73</v>
@@ -1148,7 +1243,7 @@
         <v>249382</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1156,16 +1251,16 @@
         <v>44953</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L17" s="4">
         <v>54</v>
@@ -1174,7 +1269,7 @@
         <v>58087</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1182,16 +1277,16 @@
         <v>44953</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L18" s="4">
         <v>29</v>
@@ -1200,7 +1295,7 @@
         <v>15135</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1208,22 +1303,22 @@
         <v>44953</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>18</v>
+      <c r="E19" t="s">
+        <v>114</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L19" s="3">
         <v>29</v>
@@ -1232,7 +1327,7 @@
         <v>14069</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1340,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1271,7 +1366,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1279,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1300,7 +1395,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -1317,16 +1412,16 @@
         <v>44953</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J4">
         <v>18</v>
@@ -1340,19 +1435,19 @@
         <v>44953</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>18</v>
@@ -1361,7 +1456,7 @@
         <v>42840</v>
       </c>
       <c r="L5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1372,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J3" sqref="J3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1388,16 +1483,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1405,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1420,7 +1509,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -1432,7 +1521,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -1449,19 +1538,19 @@
         <v>44953</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L4" s="6">
         <v>10</v>
@@ -1470,7 +1559,7 @@
         <v>69864</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1478,16 +1567,16 @@
         <v>44953</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1496,7 +1585,7 @@
         <v>14412</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1504,16 +1593,16 @@
         <v>44953</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6">
         <v>13</v>
@@ -1522,7 +1611,7 @@
         <v>80198</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1530,13 +1619,13 @@
         <v>44953</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7">
         <v>13</v>
@@ -1545,7 +1634,7 @@
         <v>76264</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1553,16 +1642,19 @@
         <v>44953</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="L8" s="3">
         <v>28</v>
@@ -1571,7 +1663,7 @@
         <v>53978</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1579,13 +1671,16 @@
         <v>44953</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L9" s="4">
         <v>9</v>
@@ -1594,7 +1689,7 @@
         <v>7362</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1602,13 +1697,16 @@
         <v>44953</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L10" s="4">
         <v>8</v>
@@ -1617,7 +1715,7 @@
         <v>57219</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1625,13 +1723,16 @@
         <v>44953</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L11" s="4">
         <v>16</v>
@@ -1640,7 +1741,7 @@
         <v>8298</v>
       </c>
       <c r="N11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1648,13 +1749,16 @@
         <v>44953</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L12" s="4">
         <v>36</v>
@@ -1663,68 +1767,194 @@
         <v>104581</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="24">
-        <v>44953</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>39</v>
+      <c r="A13" s="19">
+        <v>44953</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="I13" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" s="25">
+        <v>98</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="20">
         <v>36</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="20">
         <v>84923</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="C14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
-        <v>44953</v>
-      </c>
-      <c r="B15" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21">
+        <v>44953</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="I14" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="22">
+        <v>38</v>
+      </c>
+      <c r="M14" s="22">
+        <v>116438</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
+        <v>44954</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>111</v>
+      <c r="E15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="27">
-        <v>38</v>
-      </c>
-      <c r="M15" s="27">
-        <v>116438</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="4">
+        <v>21</v>
+      </c>
+      <c r="M15" s="4">
+        <v>18997</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15">
+        <v>44954</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="I16"/>
+      <c r="L16" s="4">
+        <v>17</v>
+      </c>
+      <c r="M16" s="4">
+        <v>9699</v>
+      </c>
+      <c r="N16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <v>44954</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="I17"/>
+      <c r="L17" s="4">
+        <v>4</v>
+      </c>
+      <c r="M17" s="4">
+        <v>9409</v>
+      </c>
+      <c r="N17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>44954</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="25"/>
+      <c r="L18" s="24">
+        <v>25</v>
+      </c>
+      <c r="M18" s="24">
+        <v>25404</v>
+      </c>
+      <c r="N18" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="15">
+        <v>44954</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="I19"/>
+      <c r="L19" s="4">
+        <v>25</v>
+      </c>
+      <c r="M19" s="4">
+        <v>32575</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="C20" s="4"/>
+      <c r="E20"/>
+      <c r="G20" s="4"/>
+      <c r="I20"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="C21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1733,37 +1963,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -1778,227 +2002,288 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15">
+        <v>44953</v>
+      </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" s="6">
+        <v>12</v>
+      </c>
+      <c r="M4" s="6">
+        <v>7199</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="6">
+        <v>12</v>
+      </c>
+      <c r="M5" s="6">
+        <v>6784</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
+        <v>44953</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="6">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6">
-        <v>7199</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L6" s="3">
+        <v>53</v>
+      </c>
+      <c r="M6" s="3">
+        <v>100845</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="6">
+        <v>53</v>
+      </c>
+      <c r="M7" s="6">
+        <v>94162</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <v>44953</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="5">
+        <v>44</v>
+      </c>
+      <c r="M8" s="5">
+        <v>102017</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="6">
+        <v>44</v>
+      </c>
+      <c r="M9" s="6">
+        <v>80731</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="J5" s="8">
-        <v>12</v>
-      </c>
-      <c r="K5" s="8">
-        <v>6784</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6">
-        <v>53</v>
-      </c>
-      <c r="K6">
-        <v>100845</v>
-      </c>
-      <c r="L6" s="4" t="s">
+    </row>
+    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="4">
+        <v>31</v>
+      </c>
+      <c r="M10" s="4">
+        <v>47190</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="15">
+        <v>44953</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="4">
+        <v>31</v>
+      </c>
+      <c r="M11" s="4">
+        <v>37785</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="8">
-        <v>53</v>
-      </c>
-      <c r="K7" s="8">
-        <v>94162</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="4">
-        <v>44</v>
-      </c>
-      <c r="K8" s="4">
-        <v>102017</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="6">
-        <v>44</v>
-      </c>
-      <c r="K9" s="6">
-        <v>80731</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J10" s="4">
-        <v>31</v>
-      </c>
-      <c r="K10" s="4">
-        <v>47190</v>
-      </c>
-      <c r="L10" s="4" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="21">
+        <v>44954</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I11" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="4">
-        <v>31</v>
-      </c>
-      <c r="K11" s="4">
-        <v>37785</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" s="16">
+      <c r="K13" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="16">
         <v>64</v>
       </c>
-      <c r="K14" s="16">
-        <v>125353</v>
+      <c r="M13" s="16">
+        <v>125398</v>
       </c>
     </row>
   </sheetData>
@@ -2008,266 +2293,603 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" style="27"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="6.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.6328125" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="26"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
+      <c r="B3" s="26" t="s">
+        <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17">
+        <v>44953</v>
+      </c>
+      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" s="10">
+        <v>31</v>
+      </c>
+      <c r="P4" s="10">
+        <v>13071</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="33">
+        <v>44953</v>
+      </c>
+      <c r="B5" s="31">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="12">
+        <v>31</v>
+      </c>
+      <c r="P5" s="35">
+        <v>12345</v>
+      </c>
+      <c r="Q5" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18">
+        <v>44953</v>
+      </c>
+      <c r="B6" s="29">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="3">
+        <v>19</v>
+      </c>
+      <c r="P6" s="3">
+        <v>7742</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>44953</v>
+      </c>
+      <c r="B7" s="31">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7">
+        <v>19</v>
+      </c>
+      <c r="P7">
+        <v>7231</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
+        <v>44953</v>
+      </c>
+      <c r="B8" s="29">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="O8" s="3">
+        <v>25</v>
+      </c>
+      <c r="P8" s="3">
+        <v>8889</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
+        <v>44953</v>
+      </c>
+      <c r="B9" s="31">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="H9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="N9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="6">
+        <v>25</v>
+      </c>
+      <c r="P9" s="6">
+        <v>8324</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18">
+        <v>44953</v>
+      </c>
+      <c r="B10" s="29">
         <v>7</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" s="3">
+        <v>28</v>
+      </c>
+      <c r="P10" s="3">
+        <v>10239</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <v>44954</v>
+      </c>
+      <c r="B11" s="30">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="3">
+        <v>24</v>
+      </c>
+      <c r="P11" s="3">
+        <v>5745</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>44954</v>
+      </c>
+      <c r="B12" s="32">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="4">
+        <v>24</v>
+      </c>
+      <c r="P12" s="4">
+        <v>5903</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="15">
+        <v>44955</v>
+      </c>
+      <c r="B13" s="32">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="4">
+        <v>26</v>
+      </c>
+      <c r="P13" s="4">
+        <v>6756</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="15">
+        <v>44956</v>
+      </c>
+      <c r="B14" s="32">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="4">
+        <v>27</v>
+      </c>
+      <c r="P14" s="4">
+        <v>10218</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
+        <v>44957</v>
+      </c>
+      <c r="B15" s="32">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O15" s="4">
+        <v>27</v>
+      </c>
+      <c r="P15" s="4">
+        <v>10723</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="15">
+        <v>44958</v>
+      </c>
+      <c r="B16" s="32">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="4">
+        <v>26</v>
+      </c>
+      <c r="P16" s="4">
+        <v>7451</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <v>44959</v>
+      </c>
+      <c r="B17" s="32">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="4">
+        <v>27</v>
+      </c>
+      <c r="P17" s="4">
+        <v>7580</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="15">
+        <v>44960</v>
+      </c>
+      <c r="B18" s="32">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17">
-        <v>44953</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="10">
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="4">
+        <v>27</v>
+      </c>
+      <c r="P18" s="4">
+        <v>7746</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="15">
+        <v>44961</v>
+      </c>
+      <c r="B19" s="32">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="4">
         <v>31</v>
       </c>
-      <c r="M4" s="10">
-        <v>13071</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19">
-        <v>44953</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="23">
-        <v>31</v>
-      </c>
-      <c r="M5" s="22">
-        <v>12345</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
-        <v>44953</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L6" s="3">
-        <v>19</v>
-      </c>
-      <c r="M6" s="3">
-        <v>7742</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="17">
-        <v>44953</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K7" t="s">
-        <v>99</v>
-      </c>
-      <c r="L7">
-        <v>19</v>
-      </c>
-      <c r="M7">
-        <v>7231</v>
-      </c>
-      <c r="N7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="18">
-        <v>44953</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="3">
-        <v>25</v>
-      </c>
-      <c r="M8" s="3">
-        <v>8889</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17">
-        <v>44953</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="6">
-        <v>25</v>
-      </c>
-      <c r="M9" s="6">
-        <v>8324</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18">
-        <v>44953</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L10" s="3">
-        <v>28</v>
-      </c>
-      <c r="M10" s="3">
-        <v>10239</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>107</v>
+      <c r="P19" s="4">
+        <v>9156</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>142</v>
+      </c>
+      <c r="R19" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2280,7 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
@@ -2302,7 +2924,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2310,7 +2932,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2318,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -2335,7 +2957,7 @@
         <v>44953</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>97</v>
@@ -2344,7 +2966,7 @@
         <v>296565</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish downloading WOS search results for all blocks
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -890,7 +890,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1412,7 +1412,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1536,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="L5" s="37">
-        <v>42840</v>
+        <v>42677</v>
       </c>
       <c r="M5" s="37" t="s">
         <v>92</v>
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2160,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2564,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3225,7 +3225,7 @@
         <v>37</v>
       </c>
       <c r="P21" s="36">
-        <v>18668</v>
+        <v>18673</v>
       </c>
       <c r="Q21" s="36" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
format blocked search string for scopus and delete old code that formatted for one big string - 1
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="149">
   <si>
     <t>WOS Core Collection (Bibliotheque La Perouse Access)</t>
   </si>
@@ -422,9 +422,6 @@
   </si>
   <si>
     <t>TS = ((ris* NEAR/1 "sea level$") OR "coastal flood$" OR "coastal hazard$" OR (("sea water" OR saltwater OR "salt water") NEAR/1 (incursion OR intrusion)) OR salini$ation OR aquifer$ OR (shore* NEAR/1 protect*) OR heat$stress OR "thermal stress" OR "heat wave$" OR heatwave$ OR warming OR (coral$ NEAR/1 bleaching) OR ((increas* OR ris*) NEAR/1 temperature$) OR emission$ OR carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic OR "greenhouse gas*" OR "methane" OR "fossil fuel$" OR "net zero" OR "nitrous oxide$" OR "methane" OR flurocarbon$ OR soot OR "black carbon" OR decarbon* OR "climat* change$" OR ((global OR future OR climate OR ocean) NEAR/1 (change$ OR warming)) OR "climate hazard$" OR (climate NEAR/2 variability) OR "climate extreme$" OR "extreme weather" OR "extreme event$" OR "abrupt event$" OR "coast* erosion")</t>
-  </si>
-  <si>
-    <t>NB search #31</t>
   </si>
   <si>
     <t>General CC + mitigate but missing articles: Impact of enhanced vertical mixing on marine biogeochemistry: lessons for geo-engineering and natural variability; Globalizing results from ocean in situ iron fertilization studies; Direct experiments on the ocean disposal of fossil fuel CO2</t>
@@ -918,7 +915,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1412,7 +1409,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1440,7 +1437,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1571,7 +1568,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2086,7 +2083,7 @@
         <v>25404</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.35">
@@ -2097,16 +2094,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="40" t="s">
         <v>136</v>
-      </c>
-      <c r="H19" s="40" t="s">
-        <v>137</v>
       </c>
       <c r="J19" s="40" t="s">
         <v>93</v>
@@ -2121,7 +2118,7 @@
         <v>47245</v>
       </c>
       <c r="O19" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2160,7 +2157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2180,7 +2177,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2517,7 +2514,7 @@
         <v>125398</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.35">
@@ -2528,7 +2525,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>12</v>
@@ -2537,7 +2534,7 @@
         <v>106</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J13" s="40" t="s">
         <v>88</v>
@@ -2552,7 +2549,7 @@
         <v>128467</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2562,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2587,7 +2584,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="O2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -3065,7 +3062,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>44954</v>
       </c>
@@ -3097,7 +3094,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>44954</v>
       </c>
@@ -3129,7 +3126,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>44954</v>
       </c>
@@ -3160,11 +3157,8 @@
       <c r="Q19" t="s">
         <v>131</v>
       </c>
-      <c r="R19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>44954</v>
       </c>
@@ -3172,7 +3166,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -3181,7 +3175,7 @@
         <v>132</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>88</v>
@@ -3196,10 +3190,10 @@
         <v>19106</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="35">
         <v>44954</v>
       </c>
@@ -3207,7 +3201,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F21" s="36" t="s">
         <v>36</v>
@@ -3219,7 +3213,7 @@
         <v>36</v>
       </c>
       <c r="N21" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O21" s="36">
         <v>37</v>
@@ -3228,7 +3222,7 @@
         <v>18673</v>
       </c>
       <c r="Q21" s="36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
write test list articles again to an .ris file thats compatible with upload to sysrev. Also add a readme page to the search-string-blocks.xlsx
</commit_message>
<xml_diff>
--- a/data/derived-data/search-string/search-string-blocks.xlsx
+++ b/data/derived-data/search-string/search-string-blocks.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="General options" sheetId="2" r:id="rId1"/>
-    <sheet name="Ocean renewables" sheetId="1" r:id="rId2"/>
-    <sheet name="Mitigation" sheetId="3" r:id="rId3"/>
-    <sheet name="Nature" sheetId="4" r:id="rId4"/>
-    <sheet name="Societal" sheetId="5" r:id="rId5"/>
+    <sheet name="README" sheetId="6" r:id="rId1"/>
+    <sheet name="General options" sheetId="2" r:id="rId2"/>
+    <sheet name="Ocean renewables" sheetId="1" r:id="rId3"/>
+    <sheet name="Mitigation" sheetId="3" r:id="rId4"/>
+    <sheet name="Nature" sheetId="4" r:id="rId5"/>
+    <sheet name="Societal" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="155">
   <si>
     <t>WOS Core Collection (Bibliotheque La Perouse Access)</t>
   </si>
@@ -436,9 +437,6 @@
     <t>TS = (((clean OR renew*) NEAR/5 (fuel$ OR coal OR diesel OR hydrogen OR energ* OR power OR technolog*)) OR "iron salt aerosol$" OR "methane oxidation" OR biofuel$ OR energ* OR ((efficien* OR sustainab* OR alternat*  OR electric OR decarboni?e) NEAR/5 (transport OR ship* OR biotechnolog* OR feed$ OR aquafeed$ OR (supply NEAR/2 chain$) OR product$ OR production OR material$)) OR "integrated multitrophic aquaculture" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) NEAR/15 (capture OR uptake OR remov* OR drawdown OR extract* OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea OR dispos*)) OR CCS OR DACCS OR "secure seafloor container storage" OR "bio energy" OR bioenergy OR (biomass NEAR/2 energy) OR biochar OR (bio* NEAR/2 charcoal) OR ((seaweed OR "sea weed" OR macroalga$ OR biomass OR crop$ OR log$) NEAR/2 (soil OR agriculture OR pyrolysis OR storage OR store OR sequest* OR bury OR burial OR sink* OR export* OR precipitat* OR sedimen* OR soil OR seafloor OR deep-sea)))</t>
   </si>
   <si>
-    <t>96 total</t>
-  </si>
-  <si>
     <t>TS = (((assisted OR artificial OR induced OR manage* OR restor* OR selective OR enhanc*) NEAR/5 (evolution OR adapt* OR migration OR "transgenerational acclimatization" OR breed* OR genetic OR tolerance OR resilien* OR calcification)) OR "ecosystem pushing" OR "habitat-forming species" OR (species NEAR/10 (relocat* OR translocat*)) OR ((genetic OR population OR ecological) NEAR/5 connectivity) OR "evolutionary rescue" OR "gene drive" OR (restor* NEAR/1 demograph*) OR ((probiotic$ OR phage OR viral) NEAR/1 therap*) OR "ex-situ spawn*" OR "pathogen control" OR protect* OR conserv* OR monitor* OR "climate refug*" OR "natural resource$" OR "natural capital" OR "no-regret" OR (("nature-based" OR "nature based" OR "ecosystem-based" OR "ecosystem based" OR "natural climate") NEAR/2 (solution$ OR approach* OR action$ OR measure$ OR option$)) OR ((sustainable OR "ecosystem-based" OR adaptive OR spatial OR integrated OR "natural resource" OR integrated OR fishery OR fisheries) NEAR/1 management) OR (management NEAR/1 (estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR "inter tidal" OR "sub tidal" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "sustainable ocean economic zones" OR "marine protected area$" OR MPA$ OR ((reduce OR minimize OR minimise OR decrease) AND (disturbance OR loss OR degradation OR overexploit*)) OR "environmental hardening" OR "adaptation services" OR "hybrid solution$" OR "living shoreline$" OR "nature based adaptation" OR "ecosystem based management" OR "natural climate buffer$" OR "natural climate solution$" OR "blue carbon" OR ((restor* OR translocat* OR recover* OR replant* OR rehabilitat* OR reforest* OR regener* OR reclamation OR reclaim OR rehabilitat* OR reconstruct* OR revegetat* OR re-vegetat*) NEAR/5 ("natural carbon sink$" OR estuar* OR "saline wetland$" OR coast* OR "salt marsh*" OR saltmarsh* OR "tidal marsh*" OR "tidal wetland$" OR "tidal swamp$" OR "tidal scrub" OR "tidal shrub" OR mangrove$ OR coral$ OR kelp OR macroalga$ OR seaweed OR "sea weed" OR "canopy forming algae" OR seagrass OR "sea grass" OR "algal mat$" OR "coastal vegetation" OR "sand dune$" OR reef$ OR mudflat$ OR "mussel bed" OR "blue carbon")) OR "intervention ecology" OR ((carbon OR "carbon-dioxide" OR "carbon dioxide" OR CO2 OR carbonate OR carbonic) AND (soil OR sediment)) OR depolderisation OR "eco engineering" OR "blue engineering" OR "beach nourish*" OR "shor* nourish*" OR ((restor* OR recover*) NEAR/5 (connectivity OR predator$ OR "key* species" OR tropic OR biodiversity OR "functional diversity" OR "ecosystem function")))</t>
   </si>
   <si>
@@ -470,6 +468,27 @@
   </si>
   <si>
     <t>Reine to capture missing articles</t>
+  </si>
+  <si>
+    <t>94 total</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>The complete search strategy was composed of the searching of 5 separate strings. Each string aimed to target a different part of the ORO typology.</t>
+  </si>
+  <si>
+    <t>Each sheet in the document describes the scoping searches involved in each string's refinement to optimize the retrieval of test list articles (comprehensiveness) per number of total search results (sensitivity).</t>
+  </si>
+  <si>
+    <t>Note that the test list combines articles from all different ORO types; therefore one string alone is not expected to retrieve all the test list articles.</t>
+  </si>
+  <si>
+    <t>Combined, the search results from all the search strings retrieve all the test list articles.</t>
+  </si>
+  <si>
+    <t>The row highlighted in yellow represents the search string that was finally chosen.</t>
   </si>
 </sst>
 </file>
@@ -884,10 +903,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,7 +979,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1028,7 +1092,7 @@
         <v>36</v>
       </c>
       <c r="M6">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N6">
         <v>1898637</v>
@@ -1404,12 +1468,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1437,7 +1501,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1545,12 +1609,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1568,7 +1632,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2094,7 +2158,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>12</v>
@@ -2153,12 +2217,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2177,7 +2241,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2514,7 +2578,7 @@
         <v>125398</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.35">
@@ -2525,7 +2589,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>12</v>
@@ -2534,7 +2598,7 @@
         <v>106</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J13" s="40" t="s">
         <v>88</v>
@@ -2549,7 +2613,7 @@
         <v>128467</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2557,12 +2621,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2584,7 +2648,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="O2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -3166,7 +3230,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -3175,7 +3239,7 @@
         <v>132</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>88</v>
@@ -3190,7 +3254,7 @@
         <v>19106</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -3201,7 +3265,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F21" s="36" t="s">
         <v>36</v>
@@ -3213,7 +3277,7 @@
         <v>36</v>
       </c>
       <c r="N21" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O21" s="36">
         <v>37</v>
@@ -3222,7 +3286,7 @@
         <v>18673</v>
       </c>
       <c r="Q21" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>